<commit_message>
"Các nút Nhập Xuất Excel của Sách và PX đã xong"
</commit_message>
<xml_diff>
--- a/src/Excel/Read.xlsx
+++ b/src/Excel/Read.xlsx
@@ -19,27 +19,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>STT</t>
-  </si>
-  <si>
-    <t>TÊN</t>
-  </si>
-  <si>
-    <t>TRUNG</t>
-  </si>
-  <si>
-    <t>THUẬN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KHẢI </t>
-  </si>
-  <si>
-    <t>ĐĂNG</t>
-  </si>
-  <si>
-    <t>SÚC VẬT</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Tên sách</t>
+  </si>
+  <si>
+    <t>Mã nhà xuất bản</t>
+  </si>
+  <si>
+    <t>mã tác giả</t>
+  </si>
+  <si>
+    <t>mã thể loại</t>
+  </si>
+  <si>
+    <t>số lượng tồn</t>
+  </si>
+  <si>
+    <t>năm xuất bản</t>
+  </si>
+  <si>
+    <t>đơn giá</t>
+  </si>
+  <si>
+    <t>TestExcel1</t>
+  </si>
+  <si>
+    <t>TestExcel2</t>
+  </si>
+  <si>
+    <t>TestExcel3</t>
   </si>
 </sst>
 </file>
@@ -357,60 +366,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>123</v>
+      </c>
+      <c r="F2">
+        <v>2012</v>
+      </c>
+      <c r="G2">
+        <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>123</v>
+      </c>
+      <c r="F3">
+        <v>2012</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>123</v>
+      </c>
+      <c r="F4">
+        <v>2012</v>
+      </c>
+      <c r="G4">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>